<commit_message>
Reading characters from EEPROM
</commit_message>
<xml_diff>
--- a/Font.xlsx
+++ b/Font.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>A</t>
   </si>
@@ -158,6 +158,18 @@
   <si>
     <t>width</t>
   </si>
+  <si>
+    <t>inner</t>
+  </si>
+  <si>
+    <t>with</t>
+  </si>
+  <si>
+    <t>with inner</t>
+  </si>
+  <si>
+    <t>1/2 méret szerint</t>
+  </si>
 </sst>
 </file>
 
@@ -186,7 +198,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,8 +211,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="44">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -725,11 +743,71 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -818,6 +896,93 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -830,91 +995,79 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1197,18 +1350,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BE33"/>
+  <dimension ref="A1:BO55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8:V8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="3.28515625" style="1"/>
+    <col min="1" max="8" width="3.28515625" style="1"/>
+    <col min="9" max="9" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="3.28515625" style="1"/>
+    <col min="15" max="15" width="3.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="3.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -1318,7 +1475,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1429,80 +1586,80 @@
       <c r="AW2" s="7"/>
       <c r="AX2" s="7"/>
       <c r="AY2" s="8"/>
-      <c r="BA2" s="9"/>
-      <c r="BB2" s="10"/>
-      <c r="BC2" s="10"/>
-      <c r="BD2" s="10"/>
-      <c r="BE2" s="11"/>
-    </row>
-    <row r="3" spans="1:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BA2" s="65"/>
+      <c r="BB2" s="12"/>
+      <c r="BC2" s="12"/>
+      <c r="BD2" s="12"/>
+      <c r="BE2" s="66"/>
+    </row>
+    <row r="3" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="43">
+      <c r="B3" s="31">
         <v>3</v>
       </c>
-      <c r="C3" s="44">
+      <c r="C3" s="32">
         <v>4</v>
       </c>
-      <c r="D3" s="44">
+      <c r="D3" s="32">
         <v>5</v>
       </c>
-      <c r="E3" s="44">
+      <c r="E3" s="32">
         <v>6</v>
       </c>
-      <c r="F3" s="44">
+      <c r="F3" s="32">
         <v>7</v>
       </c>
-      <c r="G3" s="44">
+      <c r="G3" s="32">
         <v>8</v>
       </c>
-      <c r="H3" s="44">
+      <c r="H3" s="32">
         <v>9</v>
       </c>
-      <c r="I3" s="44" t="s">
+      <c r="I3" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="44" t="s">
+      <c r="J3" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="44" t="s">
+      <c r="K3" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="44" t="s">
+      <c r="L3" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="44" t="s">
+      <c r="M3" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="N3" s="45" t="s">
+      <c r="N3" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="O3" s="30" t="str">
+      <c r="O3" s="59" t="str">
         <f>E2</f>
         <v>A</v>
       </c>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="31"/>
-      <c r="S3" s="31"/>
-      <c r="T3" s="31"/>
-      <c r="U3" s="31"/>
-      <c r="V3" s="31"/>
-      <c r="W3" s="31"/>
-      <c r="X3" s="31"/>
-      <c r="Y3" s="31"/>
-      <c r="Z3" s="32"/>
-      <c r="AA3" s="33" t="str">
+      <c r="P3" s="60"/>
+      <c r="Q3" s="60"/>
+      <c r="R3" s="60"/>
+      <c r="S3" s="60"/>
+      <c r="T3" s="60"/>
+      <c r="U3" s="60"/>
+      <c r="V3" s="60"/>
+      <c r="W3" s="60"/>
+      <c r="X3" s="60"/>
+      <c r="Y3" s="60"/>
+      <c r="Z3" s="61"/>
+      <c r="AA3" s="62" t="str">
         <f>F2</f>
         <v>B</v>
       </c>
-      <c r="AB3" s="31"/>
-      <c r="AC3" s="31"/>
-      <c r="AD3" s="31"/>
-      <c r="AE3" s="31"/>
-      <c r="AF3" s="31"/>
-      <c r="AG3" s="46"/>
+      <c r="AB3" s="60"/>
+      <c r="AC3" s="60"/>
+      <c r="AD3" s="60"/>
+      <c r="AE3" s="60"/>
+      <c r="AF3" s="60"/>
+      <c r="AG3" s="63"/>
       <c r="AI3" s="13"/>
       <c r="AJ3" s="14"/>
       <c r="AK3" s="14"/>
@@ -1518,60 +1675,62 @@
       <c r="AW3" s="17"/>
       <c r="AX3" s="14"/>
       <c r="AY3" s="15"/>
-      <c r="BA3" s="16"/>
-      <c r="BB3" s="17"/>
-      <c r="BC3" s="17"/>
-      <c r="BD3" s="17"/>
+      <c r="BA3" s="68"/>
+      <c r="BB3" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="BC3" s="29"/>
+      <c r="BD3" s="29"/>
       <c r="BE3" s="19"/>
     </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="30" t="str">
+      <c r="B4" s="59" t="str">
         <f>AA3</f>
         <v>B</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="33" t="str">
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="62" t="str">
         <f>G2</f>
         <v>C</v>
       </c>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35"/>
-      <c r="R4" s="36"/>
-      <c r="S4" s="34" t="str">
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="44"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="45"/>
+      <c r="S4" s="43" t="str">
         <f>H2</f>
         <v>D</v>
       </c>
-      <c r="T4" s="35"/>
-      <c r="U4" s="35"/>
-      <c r="V4" s="35"/>
-      <c r="W4" s="35"/>
-      <c r="X4" s="35"/>
-      <c r="Y4" s="35"/>
-      <c r="Z4" s="35"/>
-      <c r="AA4" s="35"/>
-      <c r="AB4" s="35"/>
-      <c r="AC4" s="35"/>
-      <c r="AD4" s="36"/>
-      <c r="AE4" s="34" t="str">
+      <c r="T4" s="44"/>
+      <c r="U4" s="44"/>
+      <c r="V4" s="44"/>
+      <c r="W4" s="44"/>
+      <c r="X4" s="44"/>
+      <c r="Y4" s="44"/>
+      <c r="Z4" s="44"/>
+      <c r="AA4" s="44"/>
+      <c r="AB4" s="44"/>
+      <c r="AC4" s="44"/>
+      <c r="AD4" s="45"/>
+      <c r="AE4" s="43" t="str">
         <f>I2</f>
         <v>E</v>
       </c>
-      <c r="AF4" s="35"/>
-      <c r="AG4" s="62"/>
+      <c r="AF4" s="44"/>
+      <c r="AG4" s="64"/>
       <c r="AI4" s="13"/>
       <c r="AJ4" s="14"/>
       <c r="AK4" s="14"/>
@@ -1587,56 +1746,58 @@
       <c r="AW4" s="17"/>
       <c r="AX4" s="17"/>
       <c r="AY4" s="15"/>
-      <c r="BA4" s="16"/>
-      <c r="BB4" s="17"/>
-      <c r="BC4" s="17"/>
-      <c r="BD4" s="17"/>
-      <c r="BE4" s="15"/>
-    </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BA4" s="68"/>
+      <c r="BB4" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="BC4" s="29"/>
+      <c r="BD4" s="29"/>
+      <c r="BE4" s="19"/>
+    </row>
+    <row r="5" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="47" t="str">
+      <c r="B5" s="40" t="str">
         <f>AE4</f>
         <v>E</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="34" t="str">
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="43" t="str">
         <f>J2</f>
         <v>F</v>
       </c>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="35"/>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="35"/>
-      <c r="S5" s="35"/>
-      <c r="T5" s="35"/>
-      <c r="U5" s="35"/>
-      <c r="V5" s="36"/>
-      <c r="W5" s="38" t="str">
+      <c r="L5" s="44"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="44"/>
+      <c r="Q5" s="44"/>
+      <c r="R5" s="44"/>
+      <c r="S5" s="44"/>
+      <c r="T5" s="44"/>
+      <c r="U5" s="44"/>
+      <c r="V5" s="45"/>
+      <c r="W5" s="46" t="str">
         <f>K2</f>
         <v>G</v>
       </c>
-      <c r="X5" s="39"/>
-      <c r="Y5" s="39"/>
-      <c r="Z5" s="39"/>
-      <c r="AA5" s="42"/>
-      <c r="AB5" s="42"/>
-      <c r="AC5" s="42"/>
-      <c r="AD5" s="42"/>
-      <c r="AE5" s="42"/>
-      <c r="AF5" s="42"/>
+      <c r="X5" s="41"/>
+      <c r="Y5" s="41"/>
+      <c r="Z5" s="41"/>
+      <c r="AA5" s="47"/>
+      <c r="AB5" s="47"/>
+      <c r="AC5" s="47"/>
+      <c r="AD5" s="47"/>
+      <c r="AE5" s="47"/>
+      <c r="AF5" s="47"/>
       <c r="AG5" s="48"/>
       <c r="AI5" s="13"/>
       <c r="AJ5" s="14"/>
@@ -1653,60 +1814,60 @@
       <c r="AW5" s="17"/>
       <c r="AX5" s="17"/>
       <c r="AY5" s="19"/>
-      <c r="BA5" s="16"/>
-      <c r="BB5" s="17"/>
-      <c r="BC5" s="17"/>
-      <c r="BD5" s="14"/>
-      <c r="BE5" s="15"/>
-    </row>
-    <row r="6" spans="1:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BA5" s="68"/>
+      <c r="BB5" s="29"/>
+      <c r="BC5" s="29"/>
+      <c r="BD5" s="29"/>
+      <c r="BE5" s="19"/>
+    </row>
+    <row r="6" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="49" t="str">
+      <c r="B6" s="34" t="str">
         <f>W5</f>
         <v>G</v>
       </c>
-      <c r="C6" s="34" t="str">
+      <c r="C6" s="43" t="str">
         <f>L2</f>
         <v>H</v>
       </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="36"/>
-      <c r="O6" s="34" t="str">
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="43" t="str">
         <f>M2</f>
         <v>I</v>
       </c>
-      <c r="P6" s="35"/>
-      <c r="Q6" s="35"/>
-      <c r="R6" s="35"/>
-      <c r="S6" s="35"/>
-      <c r="T6" s="35"/>
-      <c r="U6" s="35"/>
-      <c r="V6" s="35"/>
-      <c r="W6" s="35"/>
-      <c r="X6" s="35"/>
-      <c r="Y6" s="35"/>
-      <c r="Z6" s="36"/>
-      <c r="AA6" s="37" t="str">
+      <c r="P6" s="44"/>
+      <c r="Q6" s="44"/>
+      <c r="R6" s="44"/>
+      <c r="S6" s="44"/>
+      <c r="T6" s="44"/>
+      <c r="U6" s="44"/>
+      <c r="V6" s="44"/>
+      <c r="W6" s="44"/>
+      <c r="X6" s="44"/>
+      <c r="Y6" s="44"/>
+      <c r="Z6" s="45"/>
+      <c r="AA6" s="56" t="str">
         <f>N2</f>
         <v>J</v>
       </c>
-      <c r="AB6" s="37"/>
-      <c r="AC6" s="37"/>
-      <c r="AD6" s="37"/>
-      <c r="AE6" s="37"/>
-      <c r="AF6" s="37"/>
-      <c r="AG6" s="50"/>
+      <c r="AB6" s="56"/>
+      <c r="AC6" s="56"/>
+      <c r="AD6" s="56"/>
+      <c r="AE6" s="56"/>
+      <c r="AF6" s="56"/>
+      <c r="AG6" s="57"/>
       <c r="AI6" s="22"/>
       <c r="AJ6" s="23"/>
       <c r="AK6" s="23"/>
@@ -1722,105 +1883,105 @@
       <c r="AW6" s="26"/>
       <c r="AX6" s="26"/>
       <c r="AY6" s="27"/>
-      <c r="BA6" s="25"/>
+      <c r="BA6" s="69"/>
       <c r="BB6" s="28"/>
-      <c r="BC6" s="23"/>
-      <c r="BD6" s="23"/>
-      <c r="BE6" s="24"/>
-    </row>
-    <row r="7" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BC6" s="28"/>
+      <c r="BD6" s="28"/>
+      <c r="BE6" s="70"/>
+    </row>
+    <row r="7" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="47" t="str">
+      <c r="B7" s="40" t="str">
         <f>AA6</f>
         <v>J</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="34" t="str">
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="43" t="str">
         <f>O2</f>
         <v>K</v>
       </c>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="35"/>
-      <c r="N7" s="35"/>
-      <c r="O7" s="35"/>
-      <c r="P7" s="35"/>
-      <c r="Q7" s="35"/>
-      <c r="R7" s="36"/>
-      <c r="S7" s="34" t="str">
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="44"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="44"/>
+      <c r="Q7" s="44"/>
+      <c r="R7" s="45"/>
+      <c r="S7" s="43" t="str">
         <f>P2</f>
         <v>L</v>
       </c>
-      <c r="T7" s="35"/>
-      <c r="U7" s="35"/>
-      <c r="V7" s="35"/>
-      <c r="W7" s="35"/>
-      <c r="X7" s="35"/>
-      <c r="Y7" s="35"/>
-      <c r="Z7" s="35"/>
-      <c r="AA7" s="35"/>
-      <c r="AB7" s="35"/>
-      <c r="AC7" s="35"/>
-      <c r="AD7" s="36"/>
-      <c r="AE7" s="38" t="str">
+      <c r="T7" s="44"/>
+      <c r="U7" s="44"/>
+      <c r="V7" s="44"/>
+      <c r="W7" s="44"/>
+      <c r="X7" s="44"/>
+      <c r="Y7" s="44"/>
+      <c r="Z7" s="44"/>
+      <c r="AA7" s="44"/>
+      <c r="AB7" s="44"/>
+      <c r="AC7" s="44"/>
+      <c r="AD7" s="45"/>
+      <c r="AE7" s="46" t="str">
         <f>Q2</f>
         <v>M</v>
       </c>
-      <c r="AF7" s="39"/>
-      <c r="AG7" s="51"/>
-    </row>
-    <row r="8" spans="1:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AF7" s="41"/>
+      <c r="AG7" s="58"/>
+    </row>
+    <row r="8" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="47" t="str">
+      <c r="B8" s="40" t="str">
         <f>AE7</f>
         <v>M</v>
       </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="34" t="str">
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="43" t="str">
         <f>R2</f>
         <v>N</v>
       </c>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35"/>
-      <c r="N8" s="35"/>
-      <c r="O8" s="35"/>
-      <c r="P8" s="35"/>
-      <c r="Q8" s="35"/>
-      <c r="R8" s="35"/>
-      <c r="S8" s="35"/>
-      <c r="T8" s="35"/>
-      <c r="U8" s="35"/>
-      <c r="V8" s="36"/>
-      <c r="W8" s="38" t="str">
+      <c r="L8" s="44"/>
+      <c r="M8" s="44"/>
+      <c r="N8" s="44"/>
+      <c r="O8" s="44"/>
+      <c r="P8" s="44"/>
+      <c r="Q8" s="44"/>
+      <c r="R8" s="44"/>
+      <c r="S8" s="44"/>
+      <c r="T8" s="44"/>
+      <c r="U8" s="44"/>
+      <c r="V8" s="45"/>
+      <c r="W8" s="46" t="str">
         <f>S2</f>
         <v>O</v>
       </c>
-      <c r="X8" s="39"/>
-      <c r="Y8" s="39"/>
-      <c r="Z8" s="39"/>
-      <c r="AA8" s="42"/>
-      <c r="AB8" s="42"/>
-      <c r="AC8" s="42"/>
-      <c r="AD8" s="42"/>
-      <c r="AE8" s="42"/>
-      <c r="AF8" s="42"/>
+      <c r="X8" s="41"/>
+      <c r="Y8" s="41"/>
+      <c r="Z8" s="41"/>
+      <c r="AA8" s="47"/>
+      <c r="AB8" s="47"/>
+      <c r="AC8" s="47"/>
+      <c r="AD8" s="47"/>
+      <c r="AE8" s="47"/>
+      <c r="AF8" s="47"/>
       <c r="AG8" s="48"/>
       <c r="AI8" s="1">
         <v>4</v>
@@ -1835,651 +1996,722 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="49" t="str">
+      <c r="B9" s="34" t="str">
         <f>W8</f>
         <v>O</v>
       </c>
-      <c r="C9" s="34" t="str">
+      <c r="C9" s="43" t="str">
         <f>T2</f>
         <v>P</v>
       </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="34" t="str">
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="44"/>
+      <c r="N9" s="45"/>
+      <c r="O9" s="43" t="str">
         <f>U2</f>
         <v>Q</v>
       </c>
-      <c r="P9" s="35"/>
-      <c r="Q9" s="35"/>
-      <c r="R9" s="35"/>
-      <c r="S9" s="35"/>
-      <c r="T9" s="35"/>
-      <c r="U9" s="35"/>
-      <c r="V9" s="35"/>
-      <c r="W9" s="35"/>
-      <c r="X9" s="35"/>
-      <c r="Y9" s="35"/>
-      <c r="Z9" s="36"/>
-      <c r="AA9" s="37" t="str">
+      <c r="P9" s="44"/>
+      <c r="Q9" s="44"/>
+      <c r="R9" s="44"/>
+      <c r="S9" s="44"/>
+      <c r="T9" s="44"/>
+      <c r="U9" s="44"/>
+      <c r="V9" s="44"/>
+      <c r="W9" s="44"/>
+      <c r="X9" s="44"/>
+      <c r="Y9" s="44"/>
+      <c r="Z9" s="45"/>
+      <c r="AA9" s="56" t="str">
         <f>V2</f>
         <v>R</v>
       </c>
-      <c r="AB9" s="37"/>
-      <c r="AC9" s="37"/>
-      <c r="AD9" s="37"/>
-      <c r="AE9" s="37"/>
-      <c r="AF9" s="37"/>
-      <c r="AG9" s="50"/>
+      <c r="AB9" s="56"/>
+      <c r="AC9" s="56"/>
+      <c r="AD9" s="56"/>
+      <c r="AE9" s="56"/>
+      <c r="AF9" s="56"/>
+      <c r="AG9" s="57"/>
       <c r="AI9" s="9"/>
       <c r="AJ9" s="10"/>
       <c r="AK9" s="10"/>
       <c r="AL9" s="10"/>
       <c r="AM9" s="11"/>
-      <c r="AO9" s="6"/>
-      <c r="AP9" s="7"/>
-      <c r="AQ9" s="7"/>
-      <c r="AR9" s="7"/>
-      <c r="AS9" s="11"/>
-      <c r="AU9" s="6"/>
-      <c r="AV9" s="7"/>
-      <c r="AW9" s="7"/>
-      <c r="AX9" s="7"/>
-      <c r="AY9" s="8"/>
-      <c r="BA9" s="6"/>
-      <c r="BB9" s="7"/>
-      <c r="BC9" s="7"/>
-      <c r="BD9" s="7"/>
-      <c r="BE9" s="8"/>
-    </row>
-    <row r="10" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AO9" s="65"/>
+      <c r="AP9" s="12"/>
+      <c r="AQ9" s="12"/>
+      <c r="AR9" s="12"/>
+      <c r="AS9" s="66"/>
+      <c r="AU9" s="9"/>
+      <c r="AV9" s="10"/>
+      <c r="AW9" s="10"/>
+      <c r="AX9" s="10"/>
+      <c r="AY9" s="11"/>
+      <c r="AZ9" s="67"/>
+      <c r="BA9" s="65"/>
+      <c r="BB9" s="12"/>
+      <c r="BC9" s="12"/>
+      <c r="BD9" s="12"/>
+      <c r="BE9" s="66"/>
+    </row>
+    <row r="10" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="47" t="str">
+      <c r="B10" s="40" t="str">
         <f>AA9</f>
         <v>R</v>
       </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="34" t="str">
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="43" t="str">
         <f>W2</f>
         <v>S</v>
       </c>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
-      <c r="N10" s="35"/>
-      <c r="O10" s="35"/>
-      <c r="P10" s="35"/>
-      <c r="Q10" s="35"/>
-      <c r="R10" s="36"/>
-      <c r="S10" s="34" t="str">
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="44"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="44"/>
+      <c r="Q10" s="44"/>
+      <c r="R10" s="45"/>
+      <c r="S10" s="43" t="str">
         <f>X2</f>
         <v>T</v>
       </c>
-      <c r="T10" s="35"/>
-      <c r="U10" s="35"/>
-      <c r="V10" s="35"/>
-      <c r="W10" s="35"/>
-      <c r="X10" s="35"/>
-      <c r="Y10" s="35"/>
-      <c r="Z10" s="35"/>
-      <c r="AA10" s="35"/>
-      <c r="AB10" s="35"/>
-      <c r="AC10" s="35"/>
-      <c r="AD10" s="36"/>
-      <c r="AE10" s="38" t="str">
+      <c r="T10" s="44"/>
+      <c r="U10" s="44"/>
+      <c r="V10" s="44"/>
+      <c r="W10" s="44"/>
+      <c r="X10" s="44"/>
+      <c r="Y10" s="44"/>
+      <c r="Z10" s="44"/>
+      <c r="AA10" s="44"/>
+      <c r="AB10" s="44"/>
+      <c r="AC10" s="44"/>
+      <c r="AD10" s="45"/>
+      <c r="AE10" s="46" t="str">
         <f>Y2</f>
         <v>U</v>
       </c>
-      <c r="AF10" s="39"/>
-      <c r="AG10" s="51"/>
-      <c r="AI10" s="13"/>
+      <c r="AF10" s="41"/>
+      <c r="AG10" s="58"/>
+      <c r="AI10" s="16"/>
       <c r="AJ10" s="17"/>
       <c r="AK10" s="17"/>
       <c r="AL10" s="17"/>
-      <c r="AM10" s="18"/>
-      <c r="AO10" s="13"/>
-      <c r="AP10" s="14"/>
-      <c r="AQ10" s="17"/>
-      <c r="AR10" s="17"/>
-      <c r="AS10" s="18"/>
+      <c r="AM10" s="19"/>
+      <c r="AO10" s="68"/>
+      <c r="AP10" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="AQ10" s="29"/>
+      <c r="AR10" s="29"/>
+      <c r="AS10" s="19"/>
       <c r="AU10" s="13"/>
-      <c r="AV10" s="14"/>
-      <c r="AW10" s="14"/>
-      <c r="AX10" s="14"/>
-      <c r="AY10" s="15"/>
-      <c r="BA10" s="13"/>
-      <c r="BB10" s="14"/>
-      <c r="BC10" s="14"/>
-      <c r="BD10" s="14"/>
-      <c r="BE10" s="15"/>
-    </row>
-    <row r="11" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AV10" s="17"/>
+      <c r="AW10" s="17"/>
+      <c r="AX10" s="17"/>
+      <c r="AY10" s="18"/>
+      <c r="AZ10" s="67"/>
+      <c r="BA10" s="68"/>
+      <c r="BB10" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="BC10" s="29"/>
+      <c r="BD10" s="29"/>
+      <c r="BE10" s="19"/>
+    </row>
+    <row r="11" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="47" t="str">
+      <c r="B11" s="40" t="str">
         <f>AE10</f>
         <v>U</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="34" t="str">
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="43" t="str">
         <f>Z2</f>
         <v>V</v>
       </c>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="35"/>
-      <c r="P11" s="35"/>
-      <c r="Q11" s="35"/>
-      <c r="R11" s="35"/>
-      <c r="S11" s="35"/>
-      <c r="T11" s="35"/>
-      <c r="U11" s="35"/>
-      <c r="V11" s="36"/>
-      <c r="W11" s="38" t="str">
+      <c r="L11" s="44"/>
+      <c r="M11" s="44"/>
+      <c r="N11" s="44"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="44"/>
+      <c r="Q11" s="44"/>
+      <c r="R11" s="44"/>
+      <c r="S11" s="44"/>
+      <c r="T11" s="44"/>
+      <c r="U11" s="44"/>
+      <c r="V11" s="45"/>
+      <c r="W11" s="46" t="str">
         <f>AA2</f>
         <v>W</v>
       </c>
-      <c r="X11" s="39"/>
-      <c r="Y11" s="39"/>
-      <c r="Z11" s="39"/>
-      <c r="AA11" s="42"/>
-      <c r="AB11" s="42"/>
-      <c r="AC11" s="42"/>
-      <c r="AD11" s="42"/>
-      <c r="AE11" s="42"/>
-      <c r="AF11" s="42"/>
+      <c r="X11" s="41"/>
+      <c r="Y11" s="41"/>
+      <c r="Z11" s="41"/>
+      <c r="AA11" s="47"/>
+      <c r="AB11" s="47"/>
+      <c r="AC11" s="47"/>
+      <c r="AD11" s="47"/>
+      <c r="AE11" s="47"/>
+      <c r="AF11" s="47"/>
       <c r="AG11" s="48"/>
-      <c r="AI11" s="13"/>
+      <c r="AI11" s="16"/>
       <c r="AJ11" s="17"/>
       <c r="AK11" s="17"/>
       <c r="AL11" s="17"/>
-      <c r="AM11" s="18"/>
-      <c r="AO11" s="13"/>
-      <c r="AP11" s="17"/>
-      <c r="AQ11" s="17"/>
-      <c r="AR11" s="17"/>
-      <c r="AS11" s="18"/>
+      <c r="AM11" s="15"/>
+      <c r="AO11" s="68"/>
+      <c r="AP11" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="AQ11" s="29"/>
+      <c r="AR11" s="29"/>
+      <c r="AS11" s="19"/>
       <c r="AU11" s="13"/>
-      <c r="AV11" s="14"/>
-      <c r="AW11" s="14"/>
-      <c r="AX11" s="14"/>
-      <c r="AY11" s="15"/>
-      <c r="BA11" s="13"/>
-      <c r="BB11" s="14"/>
-      <c r="BC11" s="14"/>
-      <c r="BD11" s="14"/>
-      <c r="BE11" s="15"/>
-    </row>
-    <row r="12" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AV11" s="17"/>
+      <c r="AW11" s="17"/>
+      <c r="AX11" s="17"/>
+      <c r="AY11" s="18"/>
+      <c r="AZ11" s="67"/>
+      <c r="BA11" s="68"/>
+      <c r="BB11" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="BC11" s="29"/>
+      <c r="BD11" s="29"/>
+      <c r="BE11" s="19"/>
+    </row>
+    <row r="12" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="49" t="str">
+      <c r="B12" s="34" t="str">
         <f>W11</f>
         <v>W</v>
       </c>
-      <c r="C12" s="34" t="str">
+      <c r="C12" s="43" t="str">
         <f>AB2</f>
         <v>X</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="35"/>
-      <c r="N12" s="36"/>
-      <c r="O12" s="34" t="str">
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="44"/>
+      <c r="L12" s="44"/>
+      <c r="M12" s="44"/>
+      <c r="N12" s="45"/>
+      <c r="O12" s="43" t="str">
         <f>AC2</f>
         <v>Y</v>
       </c>
-      <c r="P12" s="35"/>
-      <c r="Q12" s="35"/>
-      <c r="R12" s="35"/>
-      <c r="S12" s="35"/>
-      <c r="T12" s="35"/>
-      <c r="U12" s="35"/>
-      <c r="V12" s="35"/>
-      <c r="W12" s="35"/>
-      <c r="X12" s="35"/>
-      <c r="Y12" s="35"/>
-      <c r="Z12" s="36"/>
-      <c r="AA12" s="37" t="str">
+      <c r="P12" s="44"/>
+      <c r="Q12" s="44"/>
+      <c r="R12" s="44"/>
+      <c r="S12" s="44"/>
+      <c r="T12" s="44"/>
+      <c r="U12" s="44"/>
+      <c r="V12" s="44"/>
+      <c r="W12" s="44"/>
+      <c r="X12" s="44"/>
+      <c r="Y12" s="44"/>
+      <c r="Z12" s="45"/>
+      <c r="AA12" s="56" t="str">
         <f>AD2</f>
         <v>Z</v>
       </c>
-      <c r="AB12" s="37"/>
-      <c r="AC12" s="37"/>
-      <c r="AD12" s="37"/>
-      <c r="AE12" s="37"/>
-      <c r="AF12" s="37"/>
-      <c r="AG12" s="50"/>
-      <c r="AI12" s="13"/>
-      <c r="AJ12" s="14"/>
+      <c r="AB12" s="56"/>
+      <c r="AC12" s="56"/>
+      <c r="AD12" s="56"/>
+      <c r="AE12" s="56"/>
+      <c r="AF12" s="56"/>
+      <c r="AG12" s="57"/>
+      <c r="AI12" s="16"/>
+      <c r="AJ12" s="17"/>
       <c r="AK12" s="17"/>
-      <c r="AL12" s="17"/>
-      <c r="AM12" s="18"/>
-      <c r="AO12" s="13"/>
-      <c r="AP12" s="17"/>
-      <c r="AQ12" s="17"/>
-      <c r="AR12" s="17"/>
-      <c r="AS12" s="18"/>
+      <c r="AL12" s="14"/>
+      <c r="AM12" s="15"/>
+      <c r="AO12" s="68"/>
+      <c r="AP12" s="29"/>
+      <c r="AQ12" s="29"/>
+      <c r="AR12" s="29"/>
+      <c r="AS12" s="19"/>
       <c r="AU12" s="13"/>
       <c r="AV12" s="14"/>
-      <c r="AW12" s="14"/>
-      <c r="AX12" s="14"/>
-      <c r="AY12" s="15"/>
-      <c r="BA12" s="13"/>
-      <c r="BB12" s="14"/>
-      <c r="BC12" s="14"/>
-      <c r="BD12" s="14"/>
-      <c r="BE12" s="15"/>
-    </row>
-    <row r="13" spans="1:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AW12" s="17"/>
+      <c r="AX12" s="17"/>
+      <c r="AY12" s="18"/>
+      <c r="AZ12" s="67"/>
+      <c r="BA12" s="68"/>
+      <c r="BB12" s="29"/>
+      <c r="BC12" s="29"/>
+      <c r="BD12" s="29"/>
+      <c r="BE12" s="19"/>
+    </row>
+    <row r="13" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="47" t="str">
+      <c r="B13" s="40" t="str">
         <f>AA12</f>
         <v>Z</v>
       </c>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="34">
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="43">
         <f>AE2</f>
         <v>0</v>
       </c>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="35"/>
-      <c r="O13" s="35"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="35"/>
-      <c r="R13" s="36"/>
-      <c r="S13" s="34">
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="44"/>
+      <c r="L13" s="44"/>
+      <c r="M13" s="44"/>
+      <c r="N13" s="44"/>
+      <c r="O13" s="44"/>
+      <c r="P13" s="44"/>
+      <c r="Q13" s="44"/>
+      <c r="R13" s="45"/>
+      <c r="S13" s="43">
         <f>AF2</f>
         <v>1</v>
       </c>
-      <c r="T13" s="35"/>
-      <c r="U13" s="35"/>
-      <c r="V13" s="35"/>
-      <c r="W13" s="35"/>
-      <c r="X13" s="35"/>
-      <c r="Y13" s="35"/>
-      <c r="Z13" s="35"/>
-      <c r="AA13" s="35"/>
-      <c r="AB13" s="35"/>
-      <c r="AC13" s="35"/>
-      <c r="AD13" s="36"/>
-      <c r="AE13" s="38">
+      <c r="T13" s="44"/>
+      <c r="U13" s="44"/>
+      <c r="V13" s="44"/>
+      <c r="W13" s="44"/>
+      <c r="X13" s="44"/>
+      <c r="Y13" s="44"/>
+      <c r="Z13" s="44"/>
+      <c r="AA13" s="44"/>
+      <c r="AB13" s="44"/>
+      <c r="AC13" s="44"/>
+      <c r="AD13" s="45"/>
+      <c r="AE13" s="46">
         <f>AG2</f>
         <v>2</v>
       </c>
-      <c r="AF13" s="39"/>
-      <c r="AG13" s="51"/>
-      <c r="AI13" s="22"/>
-      <c r="AJ13" s="23"/>
+      <c r="AF13" s="41"/>
+      <c r="AG13" s="58"/>
+      <c r="AI13" s="25"/>
+      <c r="AJ13" s="28"/>
       <c r="AK13" s="23"/>
       <c r="AL13" s="23"/>
-      <c r="AM13" s="27"/>
-      <c r="AO13" s="25"/>
-      <c r="AP13" s="26"/>
-      <c r="AQ13" s="26"/>
-      <c r="AR13" s="26"/>
-      <c r="AS13" s="27"/>
+      <c r="AM13" s="24"/>
+      <c r="AO13" s="69"/>
+      <c r="AP13" s="28"/>
+      <c r="AQ13" s="28"/>
+      <c r="AR13" s="28"/>
+      <c r="AS13" s="70"/>
       <c r="AU13" s="22"/>
       <c r="AV13" s="23"/>
       <c r="AW13" s="23"/>
       <c r="AX13" s="23"/>
-      <c r="AY13" s="24"/>
-      <c r="BA13" s="22"/>
-      <c r="BB13" s="23"/>
-      <c r="BC13" s="23"/>
-      <c r="BD13" s="23"/>
-      <c r="BE13" s="24"/>
-    </row>
-    <row r="14" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AY13" s="27"/>
+      <c r="AZ13" s="67"/>
+      <c r="BA13" s="69"/>
+      <c r="BB13" s="28"/>
+      <c r="BC13" s="28"/>
+      <c r="BD13" s="28"/>
+      <c r="BE13" s="70"/>
+    </row>
+    <row r="14" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="47">
+      <c r="B14" s="40">
         <f>AE13</f>
         <v>2</v>
       </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="34">
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="43">
         <f>B3</f>
         <v>3</v>
       </c>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
-      <c r="R14" s="35"/>
-      <c r="S14" s="35"/>
-      <c r="T14" s="35"/>
-      <c r="U14" s="35"/>
-      <c r="V14" s="36"/>
-      <c r="W14" s="38">
+      <c r="L14" s="44"/>
+      <c r="M14" s="44"/>
+      <c r="N14" s="44"/>
+      <c r="O14" s="44"/>
+      <c r="P14" s="44"/>
+      <c r="Q14" s="44"/>
+      <c r="R14" s="44"/>
+      <c r="S14" s="44"/>
+      <c r="T14" s="44"/>
+      <c r="U14" s="44"/>
+      <c r="V14" s="45"/>
+      <c r="W14" s="46">
         <f>C3</f>
         <v>4</v>
       </c>
-      <c r="X14" s="39"/>
-      <c r="Y14" s="39"/>
-      <c r="Z14" s="39"/>
-      <c r="AA14" s="42"/>
-      <c r="AB14" s="42"/>
-      <c r="AC14" s="42"/>
-      <c r="AD14" s="42"/>
-      <c r="AE14" s="42"/>
-      <c r="AF14" s="42"/>
+      <c r="X14" s="41"/>
+      <c r="Y14" s="41"/>
+      <c r="Z14" s="41"/>
+      <c r="AA14" s="47"/>
+      <c r="AB14" s="47"/>
+      <c r="AC14" s="47"/>
+      <c r="AD14" s="47"/>
+      <c r="AE14" s="47"/>
+      <c r="AF14" s="47"/>
       <c r="AG14" s="48"/>
     </row>
-    <row r="15" spans="1:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="49">
+      <c r="B15" s="34">
         <f>W14</f>
         <v>4</v>
       </c>
-      <c r="C15" s="34">
+      <c r="C15" s="43">
         <f>D3</f>
         <v>5</v>
       </c>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="36"/>
-      <c r="O15" s="34">
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="44"/>
+      <c r="M15" s="44"/>
+      <c r="N15" s="45"/>
+      <c r="O15" s="43">
         <f>E3</f>
         <v>6</v>
       </c>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="35"/>
-      <c r="R15" s="35"/>
-      <c r="S15" s="35"/>
-      <c r="T15" s="35"/>
-      <c r="U15" s="35"/>
-      <c r="V15" s="35"/>
-      <c r="W15" s="35"/>
-      <c r="X15" s="35"/>
-      <c r="Y15" s="35"/>
-      <c r="Z15" s="36"/>
-      <c r="AA15" s="37">
+      <c r="P15" s="44"/>
+      <c r="Q15" s="44"/>
+      <c r="R15" s="44"/>
+      <c r="S15" s="44"/>
+      <c r="T15" s="44"/>
+      <c r="U15" s="44"/>
+      <c r="V15" s="44"/>
+      <c r="W15" s="44"/>
+      <c r="X15" s="44"/>
+      <c r="Y15" s="44"/>
+      <c r="Z15" s="45"/>
+      <c r="AA15" s="56">
         <f>F3</f>
         <v>7</v>
       </c>
-      <c r="AB15" s="37"/>
-      <c r="AC15" s="37"/>
-      <c r="AD15" s="37"/>
-      <c r="AE15" s="37"/>
-      <c r="AF15" s="37"/>
-      <c r="AG15" s="50"/>
-      <c r="AI15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AK15" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AB15" s="56"/>
+      <c r="AC15" s="56"/>
+      <c r="AD15" s="56"/>
+      <c r="AE15" s="56"/>
+      <c r="AF15" s="56"/>
+      <c r="AG15" s="57"/>
+      <c r="AI15" s="1">
+        <v>8</v>
+      </c>
+      <c r="AO15" s="1">
+        <v>9</v>
+      </c>
+      <c r="AU15" s="1">
+        <v>10</v>
+      </c>
+      <c r="BF15" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="47">
+      <c r="B16" s="40">
         <f>AA15</f>
         <v>7</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="34">
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="43">
         <f>G3</f>
         <v>8</v>
       </c>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="35"/>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="35"/>
-      <c r="R16" s="36"/>
-      <c r="S16" s="34">
+      <c r="H16" s="44"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="44"/>
+      <c r="M16" s="44"/>
+      <c r="N16" s="44"/>
+      <c r="O16" s="44"/>
+      <c r="P16" s="44"/>
+      <c r="Q16" s="44"/>
+      <c r="R16" s="45"/>
+      <c r="S16" s="43">
         <f>H3</f>
         <v>9</v>
       </c>
-      <c r="T16" s="35"/>
-      <c r="U16" s="35"/>
-      <c r="V16" s="35"/>
-      <c r="W16" s="35"/>
-      <c r="X16" s="35"/>
-      <c r="Y16" s="35"/>
-      <c r="Z16" s="35"/>
-      <c r="AA16" s="35"/>
-      <c r="AB16" s="35"/>
-      <c r="AC16" s="35"/>
-      <c r="AD16" s="36"/>
-      <c r="AE16" s="38" t="str">
+      <c r="T16" s="44"/>
+      <c r="U16" s="44"/>
+      <c r="V16" s="44"/>
+      <c r="W16" s="44"/>
+      <c r="X16" s="44"/>
+      <c r="Y16" s="44"/>
+      <c r="Z16" s="44"/>
+      <c r="AA16" s="44"/>
+      <c r="AB16" s="44"/>
+      <c r="AC16" s="44"/>
+      <c r="AD16" s="45"/>
+      <c r="AE16" s="46" t="str">
         <f>I3</f>
         <v>.</v>
       </c>
-      <c r="AF16" s="39"/>
-      <c r="AG16" s="51"/>
-      <c r="AI16" s="6">
-        <v>0</v>
-      </c>
-      <c r="AJ16" s="7">
-        <v>3</v>
-      </c>
-      <c r="AK16" s="7">
-        <v>5</v>
-      </c>
-      <c r="AL16" s="7">
-        <v>8</v>
-      </c>
-      <c r="AM16" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AF16" s="41"/>
+      <c r="AG16" s="58"/>
+      <c r="AI16" s="6"/>
+      <c r="AJ16" s="7"/>
+      <c r="AK16" s="7"/>
+      <c r="AL16" s="7"/>
+      <c r="AM16" s="11"/>
+      <c r="AN16" s="67"/>
+      <c r="AO16" s="65"/>
+      <c r="AP16" s="12"/>
+      <c r="AQ16" s="12"/>
+      <c r="AR16" s="12"/>
+      <c r="AS16" s="66"/>
+      <c r="AU16" s="9"/>
+      <c r="AV16" s="10"/>
+      <c r="AW16" s="10"/>
+      <c r="AX16" s="10"/>
+      <c r="AY16" s="10"/>
+      <c r="AZ16" s="7"/>
+      <c r="BA16" s="7"/>
+      <c r="BB16" s="7"/>
+      <c r="BC16" s="7"/>
+      <c r="BD16" s="8"/>
+      <c r="BF16" s="6"/>
+      <c r="BG16" s="7"/>
+      <c r="BH16" s="7"/>
+      <c r="BI16" s="7"/>
+      <c r="BJ16" s="7"/>
+      <c r="BK16" s="80"/>
+      <c r="BL16" s="80"/>
+      <c r="BM16" s="80"/>
+      <c r="BN16" s="80"/>
+      <c r="BO16" s="87"/>
+    </row>
+    <row r="17" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="47" t="str">
+      <c r="B17" s="40" t="str">
         <f>AE16</f>
         <v>.</v>
       </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="34" t="str">
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="43" t="str">
         <f>J3</f>
         <v>*</v>
       </c>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="35"/>
-      <c r="S17" s="35"/>
-      <c r="T17" s="35"/>
-      <c r="U17" s="35"/>
-      <c r="V17" s="36"/>
-      <c r="W17" s="38" t="str">
+      <c r="L17" s="44"/>
+      <c r="M17" s="44"/>
+      <c r="N17" s="44"/>
+      <c r="O17" s="44"/>
+      <c r="P17" s="44"/>
+      <c r="Q17" s="44"/>
+      <c r="R17" s="44"/>
+      <c r="S17" s="44"/>
+      <c r="T17" s="44"/>
+      <c r="U17" s="44"/>
+      <c r="V17" s="45"/>
+      <c r="W17" s="46" t="str">
         <f>K3</f>
         <v>%</v>
       </c>
-      <c r="X17" s="39"/>
-      <c r="Y17" s="39"/>
-      <c r="Z17" s="39"/>
-      <c r="AA17" s="42"/>
-      <c r="AB17" s="42"/>
-      <c r="AC17" s="42"/>
-      <c r="AD17" s="42"/>
-      <c r="AE17" s="42"/>
-      <c r="AF17" s="42"/>
+      <c r="X17" s="41"/>
+      <c r="Y17" s="41"/>
+      <c r="Z17" s="41"/>
+      <c r="AA17" s="47"/>
+      <c r="AB17" s="47"/>
+      <c r="AC17" s="47"/>
+      <c r="AD17" s="47"/>
+      <c r="AE17" s="47"/>
+      <c r="AF17" s="47"/>
       <c r="AG17" s="48"/>
-      <c r="AI17" s="13">
-        <v>1</v>
-      </c>
-      <c r="AJ17" s="14">
-        <v>3</v>
-      </c>
-      <c r="AK17" s="14">
-        <v>6</v>
-      </c>
-      <c r="AL17" s="29">
-        <v>8</v>
-      </c>
-      <c r="AM17" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AI17" s="13"/>
+      <c r="AJ17" s="14"/>
+      <c r="AK17" s="17"/>
+      <c r="AL17" s="17"/>
+      <c r="AM17" s="18"/>
+      <c r="AN17" s="67"/>
+      <c r="AO17" s="68"/>
+      <c r="AP17" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="AQ17" s="29"/>
+      <c r="AR17" s="29"/>
+      <c r="AS17" s="19"/>
+      <c r="AU17" s="16"/>
+      <c r="AV17" s="17"/>
+      <c r="AW17" s="17"/>
+      <c r="AX17" s="17"/>
+      <c r="AY17" s="17"/>
+      <c r="AZ17" s="17"/>
+      <c r="BA17" s="36"/>
+      <c r="BB17" s="36"/>
+      <c r="BC17" s="36"/>
+      <c r="BD17" s="15"/>
+      <c r="BF17" s="13"/>
+      <c r="BG17" s="36"/>
+      <c r="BH17" s="36"/>
+      <c r="BI17" s="36"/>
+      <c r="BJ17" s="17"/>
+      <c r="BK17" s="82"/>
+      <c r="BL17" s="82"/>
+      <c r="BM17" s="82"/>
+      <c r="BN17" s="82"/>
+      <c r="BO17" s="85"/>
+    </row>
+    <row r="18" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="43" t="str">
+      <c r="B18" s="31" t="str">
         <f>W17</f>
         <v>%</v>
       </c>
-      <c r="C18" s="57" t="str">
+      <c r="C18" s="49" t="str">
         <f>L3</f>
         <v>:</v>
       </c>
-      <c r="D18" s="58"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="58"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="53"/>
-      <c r="L18" s="53"/>
-      <c r="M18" s="53"/>
-      <c r="N18" s="54"/>
-      <c r="O18" s="52" t="str">
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="51"/>
+      <c r="M18" s="51"/>
+      <c r="N18" s="52"/>
+      <c r="O18" s="53" t="str">
         <f>M3</f>
         <v>(</v>
       </c>
-      <c r="P18" s="53"/>
-      <c r="Q18" s="53"/>
-      <c r="R18" s="53"/>
-      <c r="S18" s="53"/>
-      <c r="T18" s="53"/>
-      <c r="U18" s="53"/>
-      <c r="V18" s="53"/>
-      <c r="W18" s="53"/>
-      <c r="X18" s="53"/>
-      <c r="Y18" s="53"/>
-      <c r="Z18" s="54"/>
-      <c r="AA18" s="55" t="str">
+      <c r="P18" s="51"/>
+      <c r="Q18" s="51"/>
+      <c r="R18" s="51"/>
+      <c r="S18" s="51"/>
+      <c r="T18" s="51"/>
+      <c r="U18" s="51"/>
+      <c r="V18" s="51"/>
+      <c r="W18" s="51"/>
+      <c r="X18" s="51"/>
+      <c r="Y18" s="51"/>
+      <c r="Z18" s="52"/>
+      <c r="AA18" s="54" t="str">
         <f>N3</f>
         <v>)</v>
       </c>
-      <c r="AB18" s="55"/>
-      <c r="AC18" s="55"/>
-      <c r="AD18" s="55"/>
-      <c r="AE18" s="55"/>
-      <c r="AF18" s="55"/>
-      <c r="AG18" s="56"/>
-      <c r="AI18" s="13">
-        <v>1</v>
-      </c>
-      <c r="AJ18" s="14">
-        <v>4</v>
-      </c>
-      <c r="AK18" s="14">
-        <v>6</v>
-      </c>
-      <c r="AL18" s="29">
-        <v>9</v>
-      </c>
-      <c r="AM18" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AB18" s="54"/>
+      <c r="AC18" s="54"/>
+      <c r="AD18" s="54"/>
+      <c r="AE18" s="54"/>
+      <c r="AF18" s="54"/>
+      <c r="AG18" s="55"/>
+      <c r="AI18" s="13"/>
+      <c r="AJ18" s="17"/>
+      <c r="AK18" s="17"/>
+      <c r="AL18" s="17"/>
+      <c r="AM18" s="18"/>
+      <c r="AN18" s="67"/>
+      <c r="AO18" s="68"/>
+      <c r="AP18" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="AQ18" s="29"/>
+      <c r="AR18" s="29"/>
+      <c r="AS18" s="19"/>
+      <c r="AU18" s="16"/>
+      <c r="AV18" s="17"/>
+      <c r="AW18" s="17"/>
+      <c r="AX18" s="17"/>
+      <c r="AY18" s="17"/>
+      <c r="AZ18" s="17"/>
+      <c r="BA18" s="17"/>
+      <c r="BB18" s="36"/>
+      <c r="BC18" s="36"/>
+      <c r="BD18" s="15"/>
+      <c r="BF18" s="13"/>
+      <c r="BG18" s="36"/>
+      <c r="BH18" s="36"/>
+      <c r="BI18" s="17"/>
+      <c r="BJ18" s="17"/>
+      <c r="BK18" s="82"/>
+      <c r="BL18" s="82"/>
+      <c r="BM18" s="82"/>
+      <c r="BN18" s="82"/>
+      <c r="BO18" s="85"/>
+    </row>
+    <row r="19" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="59" t="str">
+      <c r="B19" s="37" t="str">
         <f>AA18</f>
         <v>)</v>
       </c>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="41"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="30"/>
       <c r="H19" s="20"/>
       <c r="I19" s="20"/>
       <c r="J19" s="20"/>
@@ -2506,23 +2738,39 @@
       <c r="AE19" s="20"/>
       <c r="AF19" s="20"/>
       <c r="AG19" s="20"/>
-      <c r="AI19" s="13">
-        <v>2</v>
-      </c>
-      <c r="AJ19" s="29">
-        <v>4</v>
-      </c>
-      <c r="AK19" s="29">
-        <v>7</v>
-      </c>
-      <c r="AL19" s="29">
-        <v>9</v>
-      </c>
-      <c r="AM19" s="15">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AI19" s="13"/>
+      <c r="AJ19" s="17"/>
+      <c r="AK19" s="17"/>
+      <c r="AL19" s="17"/>
+      <c r="AM19" s="18"/>
+      <c r="AN19" s="67"/>
+      <c r="AO19" s="68"/>
+      <c r="AP19" s="29"/>
+      <c r="AQ19" s="29"/>
+      <c r="AR19" s="29"/>
+      <c r="AS19" s="19"/>
+      <c r="AU19" s="16"/>
+      <c r="AV19" s="17"/>
+      <c r="AW19" s="17"/>
+      <c r="AX19" s="17"/>
+      <c r="AY19" s="17"/>
+      <c r="AZ19" s="17"/>
+      <c r="BA19" s="17"/>
+      <c r="BB19" s="17"/>
+      <c r="BC19" s="36"/>
+      <c r="BD19" s="15"/>
+      <c r="BF19" s="13"/>
+      <c r="BG19" s="36"/>
+      <c r="BH19" s="17"/>
+      <c r="BI19" s="17"/>
+      <c r="BJ19" s="17"/>
+      <c r="BK19" s="82"/>
+      <c r="BL19" s="82"/>
+      <c r="BM19" s="82"/>
+      <c r="BN19" s="82"/>
+      <c r="BO19" s="85"/>
+    </row>
+    <row r="20" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2558,23 +2806,39 @@
       <c r="AE20" s="21"/>
       <c r="AF20" s="21"/>
       <c r="AG20" s="21"/>
-      <c r="AI20" s="22">
-        <v>2</v>
-      </c>
-      <c r="AJ20" s="23">
-        <v>5</v>
-      </c>
-      <c r="AK20" s="23">
-        <v>7</v>
-      </c>
-      <c r="AL20" s="23">
-        <v>10</v>
-      </c>
-      <c r="AM20" s="24">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AI20" s="25"/>
+      <c r="AJ20" s="26"/>
+      <c r="AK20" s="26"/>
+      <c r="AL20" s="26"/>
+      <c r="AM20" s="27"/>
+      <c r="AN20" s="67"/>
+      <c r="AO20" s="69"/>
+      <c r="AP20" s="28"/>
+      <c r="AQ20" s="28"/>
+      <c r="AR20" s="28"/>
+      <c r="AS20" s="70"/>
+      <c r="AU20" s="16"/>
+      <c r="AV20" s="17"/>
+      <c r="AW20" s="17"/>
+      <c r="AX20" s="17"/>
+      <c r="AY20" s="17"/>
+      <c r="AZ20" s="17"/>
+      <c r="BA20" s="17"/>
+      <c r="BB20" s="17"/>
+      <c r="BC20" s="17"/>
+      <c r="BD20" s="15"/>
+      <c r="BF20" s="13"/>
+      <c r="BG20" s="17"/>
+      <c r="BH20" s="17"/>
+      <c r="BI20" s="17"/>
+      <c r="BJ20" s="17"/>
+      <c r="BK20" s="82"/>
+      <c r="BL20" s="82"/>
+      <c r="BM20" s="82"/>
+      <c r="BN20" s="82"/>
+      <c r="BO20" s="85"/>
+    </row>
+    <row r="21" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2610,10 +2874,29 @@
       <c r="AE21" s="21"/>
       <c r="AF21" s="21"/>
       <c r="AG21" s="21"/>
-      <c r="AM21" s="29"/>
-      <c r="AN21" s="14"/>
-    </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AT21" s="67"/>
+      <c r="AU21" s="13"/>
+      <c r="AV21" s="17"/>
+      <c r="AW21" s="17"/>
+      <c r="AX21" s="17"/>
+      <c r="AY21" s="17"/>
+      <c r="AZ21" s="82"/>
+      <c r="BA21" s="82"/>
+      <c r="BB21" s="82"/>
+      <c r="BC21" s="82"/>
+      <c r="BD21" s="85"/>
+      <c r="BF21" s="16"/>
+      <c r="BG21" s="17"/>
+      <c r="BH21" s="17"/>
+      <c r="BI21" s="17"/>
+      <c r="BJ21" s="17"/>
+      <c r="BK21" s="17"/>
+      <c r="BL21" s="17"/>
+      <c r="BM21" s="17"/>
+      <c r="BN21" s="17"/>
+      <c r="BO21" s="15"/>
+    </row>
+    <row r="22" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2649,8 +2932,29 @@
       <c r="AE22" s="21"/>
       <c r="AF22" s="21"/>
       <c r="AG22" s="21"/>
-    </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AT22" s="67"/>
+      <c r="AU22" s="13"/>
+      <c r="AV22" s="36"/>
+      <c r="AW22" s="17"/>
+      <c r="AX22" s="17"/>
+      <c r="AY22" s="17"/>
+      <c r="AZ22" s="82"/>
+      <c r="BA22" s="82"/>
+      <c r="BB22" s="82"/>
+      <c r="BC22" s="82"/>
+      <c r="BD22" s="85"/>
+      <c r="BF22" s="16"/>
+      <c r="BG22" s="17"/>
+      <c r="BH22" s="17"/>
+      <c r="BI22" s="17"/>
+      <c r="BJ22" s="17"/>
+      <c r="BK22" s="17"/>
+      <c r="BL22" s="17"/>
+      <c r="BM22" s="17"/>
+      <c r="BN22" s="36"/>
+      <c r="BO22" s="15"/>
+    </row>
+    <row r="23" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2686,8 +2990,29 @@
       <c r="AE23" s="21"/>
       <c r="AF23" s="21"/>
       <c r="AG23" s="21"/>
-    </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AT23" s="67"/>
+      <c r="AU23" s="13"/>
+      <c r="AV23" s="36"/>
+      <c r="AW23" s="36"/>
+      <c r="AX23" s="17"/>
+      <c r="AY23" s="17"/>
+      <c r="AZ23" s="82"/>
+      <c r="BA23" s="82"/>
+      <c r="BB23" s="82"/>
+      <c r="BC23" s="82"/>
+      <c r="BD23" s="85"/>
+      <c r="BF23" s="16"/>
+      <c r="BG23" s="17"/>
+      <c r="BH23" s="17"/>
+      <c r="BI23" s="17"/>
+      <c r="BJ23" s="17"/>
+      <c r="BK23" s="17"/>
+      <c r="BL23" s="17"/>
+      <c r="BM23" s="36"/>
+      <c r="BN23" s="36"/>
+      <c r="BO23" s="15"/>
+    </row>
+    <row r="24" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2723,8 +3048,29 @@
       <c r="AE24" s="21"/>
       <c r="AF24" s="21"/>
       <c r="AG24" s="21"/>
-    </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AT24" s="67"/>
+      <c r="AU24" s="13"/>
+      <c r="AV24" s="36"/>
+      <c r="AW24" s="36"/>
+      <c r="AX24" s="36"/>
+      <c r="AY24" s="17"/>
+      <c r="AZ24" s="82"/>
+      <c r="BA24" s="82"/>
+      <c r="BB24" s="82"/>
+      <c r="BC24" s="82"/>
+      <c r="BD24" s="85"/>
+      <c r="BF24" s="16"/>
+      <c r="BG24" s="17"/>
+      <c r="BH24" s="17"/>
+      <c r="BI24" s="17"/>
+      <c r="BJ24" s="17"/>
+      <c r="BK24" s="17"/>
+      <c r="BL24" s="36"/>
+      <c r="BM24" s="36"/>
+      <c r="BN24" s="36"/>
+      <c r="BO24" s="15"/>
+    </row>
+    <row r="25" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2760,8 +3106,29 @@
       <c r="AE25" s="21"/>
       <c r="AF25" s="21"/>
       <c r="AG25" s="21"/>
-    </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AT25" s="67"/>
+      <c r="AU25" s="22"/>
+      <c r="AV25" s="35"/>
+      <c r="AW25" s="35"/>
+      <c r="AX25" s="35"/>
+      <c r="AY25" s="35"/>
+      <c r="AZ25" s="84"/>
+      <c r="BA25" s="84"/>
+      <c r="BB25" s="84"/>
+      <c r="BC25" s="84"/>
+      <c r="BD25" s="86"/>
+      <c r="BF25" s="25"/>
+      <c r="BG25" s="26"/>
+      <c r="BH25" s="26"/>
+      <c r="BI25" s="26"/>
+      <c r="BJ25" s="26"/>
+      <c r="BK25" s="35"/>
+      <c r="BL25" s="35"/>
+      <c r="BM25" s="35"/>
+      <c r="BN25" s="35"/>
+      <c r="BO25" s="24"/>
+    </row>
+    <row r="26" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2797,8 +3164,31 @@
       <c r="AE26" s="21"/>
       <c r="AF26" s="21"/>
       <c r="AG26" s="21"/>
-    </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AI26" s="67"/>
+      <c r="AJ26" s="67"/>
+      <c r="AK26" s="67"/>
+      <c r="AL26" s="67"/>
+      <c r="AM26" s="67"/>
+      <c r="AN26" s="67"/>
+      <c r="AO26" s="67"/>
+      <c r="AP26" s="67"/>
+      <c r="AQ26" s="67"/>
+      <c r="AR26" s="67"/>
+      <c r="AS26" s="67"/>
+      <c r="AT26" s="67"/>
+      <c r="AU26" s="67"/>
+      <c r="AV26" s="67"/>
+      <c r="AW26" s="67"/>
+      <c r="AX26" s="67"/>
+      <c r="AY26" s="67"/>
+      <c r="AZ26" s="67"/>
+      <c r="BA26" s="67"/>
+      <c r="BB26" s="67"/>
+      <c r="BC26" s="67"/>
+      <c r="BD26" s="67"/>
+      <c r="BE26" s="67"/>
+    </row>
+    <row r="27" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2834,8 +3224,33 @@
       <c r="AE27" s="21"/>
       <c r="AF27" s="21"/>
       <c r="AG27" s="21"/>
-    </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AI27" s="67">
+        <v>12</v>
+      </c>
+      <c r="AJ27" s="71" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK27" s="71"/>
+      <c r="AL27" s="71"/>
+      <c r="AM27" s="71"/>
+      <c r="AN27" s="67"/>
+      <c r="AO27" s="67">
+        <v>13</v>
+      </c>
+      <c r="AP27" s="78" t="s">
+        <v>36</v>
+      </c>
+      <c r="AR27" s="67"/>
+      <c r="AS27" s="67"/>
+      <c r="AT27" s="67"/>
+      <c r="AU27" s="1">
+        <v>14</v>
+      </c>
+      <c r="BF27" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2871,8 +3286,40 @@
       <c r="AE28" s="21"/>
       <c r="AF28" s="21"/>
       <c r="AG28" s="21"/>
-    </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AI28" s="9"/>
+      <c r="AJ28" s="10"/>
+      <c r="AK28" s="10"/>
+      <c r="AL28" s="10"/>
+      <c r="AM28" s="11"/>
+      <c r="AN28" s="67"/>
+      <c r="AO28" s="9"/>
+      <c r="AP28" s="12"/>
+      <c r="AQ28" s="7"/>
+      <c r="AR28" s="7"/>
+      <c r="AS28" s="8"/>
+      <c r="AT28" s="67"/>
+      <c r="AU28" s="79"/>
+      <c r="AV28" s="80"/>
+      <c r="AW28" s="80"/>
+      <c r="AX28" s="80"/>
+      <c r="AY28" s="80"/>
+      <c r="AZ28" s="7"/>
+      <c r="BA28" s="7"/>
+      <c r="BB28" s="7"/>
+      <c r="BC28" s="7"/>
+      <c r="BD28" s="8"/>
+      <c r="BF28" s="6"/>
+      <c r="BG28" s="7"/>
+      <c r="BH28" s="7"/>
+      <c r="BI28" s="7"/>
+      <c r="BJ28" s="7"/>
+      <c r="BK28" s="10"/>
+      <c r="BL28" s="10"/>
+      <c r="BM28" s="10"/>
+      <c r="BN28" s="10"/>
+      <c r="BO28" s="11"/>
+    </row>
+    <row r="29" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2908,8 +3355,40 @@
       <c r="AE29" s="21"/>
       <c r="AF29" s="21"/>
       <c r="AG29" s="21"/>
-    </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AI29" s="16"/>
+      <c r="AJ29" s="17"/>
+      <c r="AK29" s="17"/>
+      <c r="AL29" s="17"/>
+      <c r="AM29" s="19"/>
+      <c r="AN29" s="67"/>
+      <c r="AO29" s="16"/>
+      <c r="AP29" s="17"/>
+      <c r="AQ29" s="17"/>
+      <c r="AR29" s="36"/>
+      <c r="AS29" s="15"/>
+      <c r="AT29" s="67"/>
+      <c r="AU29" s="81"/>
+      <c r="AV29" s="82"/>
+      <c r="AW29" s="82"/>
+      <c r="AX29" s="82"/>
+      <c r="AY29" s="82"/>
+      <c r="AZ29" s="17"/>
+      <c r="BA29" s="36"/>
+      <c r="BB29" s="36"/>
+      <c r="BC29" s="36"/>
+      <c r="BD29" s="15"/>
+      <c r="BF29" s="13"/>
+      <c r="BG29" s="36"/>
+      <c r="BH29" s="36"/>
+      <c r="BI29" s="36"/>
+      <c r="BJ29" s="17"/>
+      <c r="BK29" s="17"/>
+      <c r="BL29" s="17"/>
+      <c r="BM29" s="17"/>
+      <c r="BN29" s="17"/>
+      <c r="BO29" s="18"/>
+    </row>
+    <row r="30" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2945,8 +3424,40 @@
       <c r="AE30" s="21"/>
       <c r="AF30" s="21"/>
       <c r="AG30" s="21"/>
-    </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AI30" s="16"/>
+      <c r="AJ30" s="17"/>
+      <c r="AK30" s="17"/>
+      <c r="AL30" s="29"/>
+      <c r="AM30" s="15"/>
+      <c r="AN30" s="67"/>
+      <c r="AO30" s="16"/>
+      <c r="AP30" s="17"/>
+      <c r="AQ30" s="17"/>
+      <c r="AR30" s="17"/>
+      <c r="AS30" s="15"/>
+      <c r="AT30" s="67"/>
+      <c r="AU30" s="81"/>
+      <c r="AV30" s="82"/>
+      <c r="AW30" s="82"/>
+      <c r="AX30" s="82"/>
+      <c r="AY30" s="82"/>
+      <c r="AZ30" s="17"/>
+      <c r="BA30" s="17"/>
+      <c r="BB30" s="36"/>
+      <c r="BC30" s="36"/>
+      <c r="BD30" s="15"/>
+      <c r="BF30" s="13"/>
+      <c r="BG30" s="36"/>
+      <c r="BH30" s="36"/>
+      <c r="BI30" s="17"/>
+      <c r="BJ30" s="17"/>
+      <c r="BK30" s="17"/>
+      <c r="BL30" s="17"/>
+      <c r="BM30" s="17"/>
+      <c r="BN30" s="17"/>
+      <c r="BO30" s="18"/>
+    </row>
+    <row r="31" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2982,8 +3493,40 @@
       <c r="AE31" s="21"/>
       <c r="AF31" s="21"/>
       <c r="AG31" s="21"/>
-    </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AI31" s="16"/>
+      <c r="AJ31" s="17"/>
+      <c r="AK31" s="17"/>
+      <c r="AL31" s="17"/>
+      <c r="AM31" s="15"/>
+      <c r="AN31" s="67"/>
+      <c r="AO31" s="16"/>
+      <c r="AP31" s="17"/>
+      <c r="AQ31" s="17"/>
+      <c r="AR31" s="17"/>
+      <c r="AS31" s="19"/>
+      <c r="AT31" s="67"/>
+      <c r="AU31" s="81"/>
+      <c r="AV31" s="82"/>
+      <c r="AW31" s="82"/>
+      <c r="AX31" s="82"/>
+      <c r="AY31" s="82"/>
+      <c r="AZ31" s="17"/>
+      <c r="BA31" s="17"/>
+      <c r="BB31" s="17"/>
+      <c r="BC31" s="36"/>
+      <c r="BD31" s="15"/>
+      <c r="BF31" s="13"/>
+      <c r="BG31" s="36"/>
+      <c r="BH31" s="17"/>
+      <c r="BI31" s="17"/>
+      <c r="BJ31" s="17"/>
+      <c r="BK31" s="17"/>
+      <c r="BL31" s="17"/>
+      <c r="BM31" s="17"/>
+      <c r="BN31" s="17"/>
+      <c r="BO31" s="18"/>
+    </row>
+    <row r="32" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -3019,8 +3562,40 @@
       <c r="AE32" s="21"/>
       <c r="AF32" s="21"/>
       <c r="AG32" s="21"/>
-    </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AI32" s="25"/>
+      <c r="AJ32" s="26"/>
+      <c r="AK32" s="26"/>
+      <c r="AL32" s="26"/>
+      <c r="AM32" s="27"/>
+      <c r="AN32" s="67"/>
+      <c r="AO32" s="25"/>
+      <c r="AP32" s="26"/>
+      <c r="AQ32" s="26"/>
+      <c r="AR32" s="26"/>
+      <c r="AS32" s="27"/>
+      <c r="AT32" s="67"/>
+      <c r="AU32" s="81"/>
+      <c r="AV32" s="82"/>
+      <c r="AW32" s="82"/>
+      <c r="AX32" s="82"/>
+      <c r="AY32" s="82"/>
+      <c r="AZ32" s="17"/>
+      <c r="BA32" s="17"/>
+      <c r="BB32" s="17"/>
+      <c r="BC32" s="17"/>
+      <c r="BD32" s="15"/>
+      <c r="BF32" s="13"/>
+      <c r="BG32" s="17"/>
+      <c r="BH32" s="17"/>
+      <c r="BI32" s="17"/>
+      <c r="BJ32" s="17"/>
+      <c r="BK32" s="17"/>
+      <c r="BL32" s="17"/>
+      <c r="BM32" s="17"/>
+      <c r="BN32" s="17"/>
+      <c r="BO32" s="18"/>
+    </row>
+    <row r="33" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -3056,9 +3631,862 @@
       <c r="AE33" s="21"/>
       <c r="AF33" s="21"/>
       <c r="AG33" s="21"/>
+      <c r="AU33" s="13"/>
+      <c r="AV33" s="17"/>
+      <c r="AW33" s="17"/>
+      <c r="AX33" s="17"/>
+      <c r="AY33" s="17"/>
+      <c r="AZ33" s="17"/>
+      <c r="BA33" s="17"/>
+      <c r="BB33" s="17"/>
+      <c r="BC33" s="17"/>
+      <c r="BD33" s="18"/>
+      <c r="BF33" s="81"/>
+      <c r="BG33" s="82"/>
+      <c r="BH33" s="82"/>
+      <c r="BI33" s="82"/>
+      <c r="BJ33" s="82"/>
+      <c r="BK33" s="17"/>
+      <c r="BL33" s="17"/>
+      <c r="BM33" s="17"/>
+      <c r="BN33" s="17"/>
+      <c r="BO33" s="15"/>
+    </row>
+    <row r="34" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AI34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU34" s="13"/>
+      <c r="AV34" s="36"/>
+      <c r="AW34" s="17"/>
+      <c r="AX34" s="17"/>
+      <c r="AY34" s="17"/>
+      <c r="AZ34" s="17"/>
+      <c r="BA34" s="17"/>
+      <c r="BB34" s="17"/>
+      <c r="BC34" s="17"/>
+      <c r="BD34" s="18"/>
+      <c r="BF34" s="81"/>
+      <c r="BG34" s="82"/>
+      <c r="BH34" s="82"/>
+      <c r="BI34" s="82"/>
+      <c r="BJ34" s="82"/>
+      <c r="BK34" s="17"/>
+      <c r="BL34" s="17"/>
+      <c r="BM34" s="17"/>
+      <c r="BN34" s="36"/>
+      <c r="BO34" s="15"/>
+    </row>
+    <row r="35" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="AI35" s="6">
+        <v>0</v>
+      </c>
+      <c r="AJ35" s="7">
+        <v>3</v>
+      </c>
+      <c r="AK35" s="7">
+        <v>5</v>
+      </c>
+      <c r="AL35" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM35" s="8">
+        <v>10</v>
+      </c>
+      <c r="AU35" s="13"/>
+      <c r="AV35" s="36"/>
+      <c r="AW35" s="36"/>
+      <c r="AX35" s="17"/>
+      <c r="AY35" s="17"/>
+      <c r="AZ35" s="17"/>
+      <c r="BA35" s="17"/>
+      <c r="BB35" s="17"/>
+      <c r="BC35" s="17"/>
+      <c r="BD35" s="18"/>
+      <c r="BF35" s="81"/>
+      <c r="BG35" s="82"/>
+      <c r="BH35" s="82"/>
+      <c r="BI35" s="82"/>
+      <c r="BJ35" s="82"/>
+      <c r="BK35" s="17"/>
+      <c r="BL35" s="17"/>
+      <c r="BM35" s="36"/>
+      <c r="BN35" s="36"/>
+      <c r="BO35" s="15"/>
+    </row>
+    <row r="36" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="1">
+        <v>1</v>
+      </c>
+      <c r="W36" s="1">
+        <f>I39</f>
+        <v>5</v>
+      </c>
+      <c r="AI36" s="13">
+        <v>1</v>
+      </c>
+      <c r="AJ36" s="14">
+        <v>3</v>
+      </c>
+      <c r="AK36" s="14">
+        <v>6</v>
+      </c>
+      <c r="AL36" s="29">
+        <v>8</v>
+      </c>
+      <c r="AM36" s="15">
+        <v>11</v>
+      </c>
+      <c r="AU36" s="13"/>
+      <c r="AV36" s="36"/>
+      <c r="AW36" s="36"/>
+      <c r="AX36" s="36"/>
+      <c r="AY36" s="17"/>
+      <c r="AZ36" s="17"/>
+      <c r="BA36" s="17"/>
+      <c r="BB36" s="17"/>
+      <c r="BC36" s="17"/>
+      <c r="BD36" s="18"/>
+      <c r="BF36" s="81"/>
+      <c r="BG36" s="82"/>
+      <c r="BH36" s="82"/>
+      <c r="BI36" s="82"/>
+      <c r="BJ36" s="82"/>
+      <c r="BK36" s="17"/>
+      <c r="BL36" s="36"/>
+      <c r="BM36" s="36"/>
+      <c r="BN36" s="36"/>
+      <c r="BO36" s="15"/>
+    </row>
+    <row r="37" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="6"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="8"/>
+      <c r="I37" s="72">
+        <f>C36*16+C37</f>
+        <v>16</v>
+      </c>
+      <c r="J37" s="73">
+        <f>C38*16+C39</f>
+        <v>16</v>
+      </c>
+      <c r="K37" s="74">
+        <f>C40*16+C41</f>
+        <v>16</v>
+      </c>
+      <c r="L37" s="72">
+        <f>D37*16+D38</f>
+        <v>0</v>
+      </c>
+      <c r="M37" s="73">
+        <f>D39*16+D40</f>
+        <v>0</v>
+      </c>
+      <c r="N37" s="74">
+        <f>D41*16+E37</f>
+        <v>0</v>
+      </c>
+      <c r="O37" s="72">
+        <f>E38*16+E39</f>
+        <v>0</v>
+      </c>
+      <c r="P37" s="73">
+        <f>E40*16+E41</f>
+        <v>0</v>
+      </c>
+      <c r="Q37" s="74">
+        <f>F37*16+F38</f>
+        <v>0</v>
+      </c>
+      <c r="R37" s="72">
+        <f>F39*16+F40</f>
+        <v>0</v>
+      </c>
+      <c r="S37" s="73">
+        <f>F41*16+G37</f>
+        <v>0</v>
+      </c>
+      <c r="T37" s="74">
+        <f>G38*16+G39</f>
+        <v>0</v>
+      </c>
+      <c r="U37" s="75">
+        <f>G40*16+G41</f>
+        <v>0</v>
+      </c>
+      <c r="W37" s="6">
+        <f>I40</f>
+        <v>14</v>
+      </c>
+      <c r="X37" s="7">
+        <f>L39</f>
+        <v>0</v>
+      </c>
+      <c r="Y37" s="7">
+        <f>N40</f>
+        <v>0</v>
+      </c>
+      <c r="Z37" s="7">
+        <f>Q39</f>
+        <v>0</v>
+      </c>
+      <c r="AA37" s="8">
+        <f>S40</f>
+        <v>11</v>
+      </c>
+      <c r="AI37" s="13">
+        <v>1</v>
+      </c>
+      <c r="AJ37" s="14">
+        <v>4</v>
+      </c>
+      <c r="AK37" s="14">
+        <v>6</v>
+      </c>
+      <c r="AL37" s="29">
+        <v>9</v>
+      </c>
+      <c r="AM37" s="15">
+        <v>11</v>
+      </c>
+      <c r="AU37" s="22"/>
+      <c r="AV37" s="35"/>
+      <c r="AW37" s="35"/>
+      <c r="AX37" s="35"/>
+      <c r="AY37" s="35"/>
+      <c r="AZ37" s="26"/>
+      <c r="BA37" s="26"/>
+      <c r="BB37" s="26"/>
+      <c r="BC37" s="26"/>
+      <c r="BD37" s="27"/>
+      <c r="BF37" s="83"/>
+      <c r="BG37" s="84"/>
+      <c r="BH37" s="84"/>
+      <c r="BI37" s="84"/>
+      <c r="BJ37" s="84"/>
+      <c r="BK37" s="35"/>
+      <c r="BL37" s="35"/>
+      <c r="BM37" s="35"/>
+      <c r="BN37" s="35"/>
+      <c r="BO37" s="24"/>
+    </row>
+    <row r="38" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="13">
+        <v>1</v>
+      </c>
+      <c r="D38" s="36"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="15"/>
+      <c r="I38" s="1">
+        <v>94</v>
+      </c>
+      <c r="J38" s="1">
+        <v>0</v>
+      </c>
+      <c r="K38" s="1">
+        <v>15</v>
+      </c>
+      <c r="L38" s="1">
+        <v>14</v>
+      </c>
+      <c r="M38" s="1">
+        <v>15</v>
+      </c>
+      <c r="N38" s="1">
+        <v>0</v>
+      </c>
+      <c r="O38" s="1">
+        <v>1</v>
+      </c>
+      <c r="P38" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>11</v>
+      </c>
+      <c r="R38" s="1">
+        <v>10</v>
+      </c>
+      <c r="S38" s="1">
+        <v>11</v>
+      </c>
+      <c r="T38" s="1">
+        <v>0</v>
+      </c>
+      <c r="U38" s="1">
+        <v>10</v>
+      </c>
+      <c r="W38" s="13">
+        <f>J39</f>
+        <v>0</v>
+      </c>
+      <c r="X38" s="36">
+        <f>L40</f>
+        <v>14</v>
+      </c>
+      <c r="Y38" s="36">
+        <f>O39</f>
+        <v>0</v>
+      </c>
+      <c r="Z38" s="36">
+        <f>Q40</f>
+        <v>11</v>
+      </c>
+      <c r="AA38" s="15">
+        <f>T39</f>
+        <v>0</v>
+      </c>
+      <c r="AI38" s="13">
+        <v>2</v>
+      </c>
+      <c r="AJ38" s="29">
+        <v>4</v>
+      </c>
+      <c r="AK38" s="29">
+        <v>7</v>
+      </c>
+      <c r="AL38" s="29">
+        <v>9</v>
+      </c>
+      <c r="AM38" s="15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="13"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="36"/>
+      <c r="G39" s="15"/>
+      <c r="I39" s="6">
+        <f>ROUNDDOWN(I38/16,0)</f>
+        <v>5</v>
+      </c>
+      <c r="J39" s="7">
+        <f t="shared" ref="J39:U39" si="0">ROUNDDOWN(J38/16,0)</f>
+        <v>0</v>
+      </c>
+      <c r="K39" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L39" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M39" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N39" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O39" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P39" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q39" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R39" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S39" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T39" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U39" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W39" s="13">
+        <f>J40</f>
+        <v>0</v>
+      </c>
+      <c r="X39" s="36">
+        <f>M39</f>
+        <v>0</v>
+      </c>
+      <c r="Y39" s="36">
+        <f>O40</f>
+        <v>1</v>
+      </c>
+      <c r="Z39" s="36">
+        <f>R39</f>
+        <v>0</v>
+      </c>
+      <c r="AA39" s="15">
+        <f>T40</f>
+        <v>0</v>
+      </c>
+      <c r="AI39" s="22">
+        <v>2</v>
+      </c>
+      <c r="AJ39" s="23">
+        <v>5</v>
+      </c>
+      <c r="AK39" s="23">
+        <v>7</v>
+      </c>
+      <c r="AL39" s="23">
+        <v>10</v>
+      </c>
+      <c r="AM39" s="24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="13">
+        <v>1</v>
+      </c>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="15"/>
+      <c r="I40" s="22">
+        <f>MOD(I38,16)</f>
+        <v>14</v>
+      </c>
+      <c r="J40" s="35">
+        <f t="shared" ref="J40:U40" si="1">MOD(J38,16)</f>
+        <v>0</v>
+      </c>
+      <c r="K40" s="35">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="L40" s="35">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="M40" s="35">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="N40" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O40" s="35">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P40" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q40" s="35">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="R40" s="35">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="S40" s="35">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="T40" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U40" s="24">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="V40" s="29"/>
+      <c r="W40" s="13">
+        <f>K39</f>
+        <v>0</v>
+      </c>
+      <c r="X40" s="36">
+        <f>M40</f>
+        <v>15</v>
+      </c>
+      <c r="Y40" s="36">
+        <f>P39</f>
+        <v>0</v>
+      </c>
+      <c r="Z40" s="36">
+        <f>R40</f>
+        <v>10</v>
+      </c>
+      <c r="AA40" s="15">
+        <f>U39</f>
+        <v>0</v>
+      </c>
+      <c r="AB40" s="29"/>
+      <c r="AC40" s="29"/>
+      <c r="AD40" s="29"/>
+      <c r="AE40" s="29"/>
+      <c r="AF40" s="29"/>
+      <c r="AG40" s="29"/>
+    </row>
+    <row r="41" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="22"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="24"/>
+      <c r="K41" s="29"/>
+      <c r="L41" s="29"/>
+      <c r="M41" s="29"/>
+      <c r="N41" s="29"/>
+      <c r="O41" s="29"/>
+      <c r="P41" s="29"/>
+      <c r="Q41" s="29"/>
+      <c r="R41" s="29"/>
+      <c r="S41" s="29"/>
+      <c r="T41" s="29"/>
+      <c r="U41" s="29"/>
+      <c r="V41" s="29"/>
+      <c r="W41" s="22">
+        <f>K40</f>
+        <v>15</v>
+      </c>
+      <c r="X41" s="35">
+        <f>N39</f>
+        <v>0</v>
+      </c>
+      <c r="Y41" s="35">
+        <f>P40</f>
+        <v>0</v>
+      </c>
+      <c r="Z41" s="35">
+        <f>T39</f>
+        <v>0</v>
+      </c>
+      <c r="AA41" s="24">
+        <f>U40</f>
+        <v>10</v>
+      </c>
+      <c r="AB41" s="29"/>
+      <c r="AC41" s="29"/>
+      <c r="AD41" s="29"/>
+      <c r="AE41" s="29"/>
+      <c r="AF41" s="29"/>
+      <c r="AG41" s="29"/>
+    </row>
+    <row r="42" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="K42" s="29"/>
+      <c r="L42" s="29"/>
+      <c r="M42" s="29"/>
+      <c r="N42" s="29"/>
+      <c r="O42" s="29"/>
+      <c r="P42" s="29"/>
+      <c r="Q42" s="29"/>
+      <c r="R42" s="29"/>
+      <c r="S42" s="29"/>
+      <c r="T42" s="29"/>
+      <c r="U42" s="29"/>
+      <c r="V42" s="29"/>
+      <c r="W42" s="29"/>
+      <c r="X42" s="29"/>
+      <c r="Y42" s="29"/>
+      <c r="Z42" s="29"/>
+      <c r="AA42" s="29"/>
+      <c r="AB42" s="29"/>
+      <c r="AC42" s="29"/>
+      <c r="AD42" s="29"/>
+      <c r="AE42" s="29"/>
+      <c r="AF42" s="29"/>
+      <c r="AG42" s="29"/>
+    </row>
+    <row r="43" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="B43" s="76"/>
+      <c r="C43" s="77" t="str">
+        <f>CONCATENATE("EEPROM.write(a, ",I37,"); a++;")</f>
+        <v>EEPROM.write(a, 16); a++;</v>
+      </c>
+      <c r="D43" s="77"/>
+      <c r="E43" s="77"/>
+      <c r="F43" s="77"/>
+      <c r="G43" s="77"/>
+      <c r="H43" s="77"/>
+      <c r="I43" s="77"/>
+      <c r="K43" s="29"/>
+      <c r="L43" s="29"/>
+      <c r="M43" s="29"/>
+      <c r="N43" s="29"/>
+      <c r="O43" s="29"/>
+      <c r="P43" s="29"/>
+      <c r="Q43" s="29"/>
+      <c r="R43" s="29"/>
+      <c r="S43" s="29"/>
+      <c r="T43" s="29"/>
+      <c r="U43" s="29"/>
+      <c r="V43" s="29"/>
+      <c r="W43" s="29"/>
+      <c r="X43" s="29"/>
+      <c r="Y43" s="29"/>
+      <c r="Z43" s="29"/>
+      <c r="AA43" s="29"/>
+      <c r="AB43" s="29"/>
+      <c r="AC43" s="29"/>
+      <c r="AD43" s="29"/>
+      <c r="AE43" s="29"/>
+      <c r="AF43" s="29"/>
+      <c r="AG43" s="29"/>
+    </row>
+    <row r="44" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A44" s="76"/>
+      <c r="B44" s="76"/>
+      <c r="C44" s="77" t="str">
+        <f>CONCATENATE("  EEPROM.write(a, ",J37,"); a++;")</f>
+        <v xml:space="preserve">  EEPROM.write(a, 16); a++;</v>
+      </c>
+      <c r="D44" s="77"/>
+      <c r="E44" s="77"/>
+      <c r="F44" s="77"/>
+      <c r="G44" s="77"/>
+      <c r="H44" s="77"/>
+      <c r="I44" s="77"/>
+      <c r="K44" s="29"/>
+      <c r="L44" s="29"/>
+      <c r="M44" s="29"/>
+      <c r="N44" s="29"/>
+      <c r="O44" s="29"/>
+      <c r="P44" s="29"/>
+      <c r="Q44" s="29"/>
+      <c r="R44" s="29"/>
+      <c r="S44" s="29"/>
+      <c r="T44" s="29"/>
+      <c r="U44" s="29"/>
+      <c r="V44" s="29"/>
+      <c r="W44" s="29"/>
+      <c r="X44" s="29"/>
+      <c r="Y44" s="29"/>
+      <c r="Z44" s="29"/>
+      <c r="AA44" s="29"/>
+      <c r="AB44" s="29"/>
+      <c r="AC44" s="29"/>
+      <c r="AD44" s="29"/>
+      <c r="AE44" s="29"/>
+      <c r="AF44" s="29"/>
+      <c r="AG44" s="29"/>
+    </row>
+    <row r="45" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="C45" s="77" t="str">
+        <f>CONCATENATE("  EEPROM.write(a, ",K37,"); a++;")</f>
+        <v xml:space="preserve">  EEPROM.write(a, 16); a++;</v>
+      </c>
+      <c r="D45" s="77"/>
+      <c r="E45" s="77"/>
+      <c r="F45" s="77"/>
+      <c r="G45" s="77"/>
+      <c r="H45" s="77"/>
+      <c r="I45" s="77"/>
+      <c r="K45" s="29"/>
+      <c r="L45" s="29"/>
+      <c r="M45" s="29"/>
+      <c r="N45" s="29"/>
+      <c r="O45" s="29"/>
+      <c r="P45" s="29"/>
+      <c r="Q45" s="29"/>
+      <c r="R45" s="29"/>
+      <c r="S45" s="29"/>
+      <c r="T45" s="29"/>
+      <c r="U45" s="29"/>
+      <c r="V45" s="29"/>
+      <c r="W45" s="29"/>
+      <c r="X45" s="29"/>
+      <c r="Y45" s="29"/>
+      <c r="Z45" s="29"/>
+      <c r="AA45" s="29"/>
+      <c r="AB45" s="29"/>
+      <c r="AC45" s="29"/>
+      <c r="AD45" s="29"/>
+      <c r="AE45" s="29"/>
+      <c r="AF45" s="29"/>
+      <c r="AG45" s="29"/>
+    </row>
+    <row r="46" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="C46" s="77" t="str">
+        <f>CONCATENATE("  EEPROM.write(a, ",L37,"); a++;")</f>
+        <v xml:space="preserve">  EEPROM.write(a, 0); a++;</v>
+      </c>
+      <c r="D46" s="77"/>
+      <c r="E46" s="77"/>
+      <c r="F46" s="77"/>
+      <c r="G46" s="77"/>
+      <c r="H46" s="77"/>
+      <c r="I46" s="77"/>
+    </row>
+    <row r="47" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="C47" s="77" t="str">
+        <f>CONCATENATE("  EEPROM.write(a, ",M37,"); a++;")</f>
+        <v xml:space="preserve">  EEPROM.write(a, 0); a++;</v>
+      </c>
+      <c r="D47" s="77"/>
+      <c r="E47" s="77"/>
+      <c r="F47" s="77"/>
+      <c r="G47" s="77"/>
+      <c r="H47" s="77"/>
+      <c r="I47" s="77"/>
+    </row>
+    <row r="48" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="C48" s="77" t="str">
+        <f>CONCATENATE("  EEPROM.write(a, ",N37,"); a++;")</f>
+        <v xml:space="preserve">  EEPROM.write(a, 0); a++;</v>
+      </c>
+      <c r="D48" s="77"/>
+      <c r="E48" s="77"/>
+      <c r="F48" s="77"/>
+      <c r="G48" s="77"/>
+      <c r="H48" s="77"/>
+      <c r="I48" s="77"/>
+    </row>
+    <row r="49" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C49" s="77" t="str">
+        <f>CONCATENATE("  EEPROM.write(a, ",O37,"); a++;")</f>
+        <v xml:space="preserve">  EEPROM.write(a, 0); a++;</v>
+      </c>
+      <c r="D49" s="77"/>
+      <c r="E49" s="77"/>
+      <c r="F49" s="77"/>
+      <c r="G49" s="77"/>
+      <c r="H49" s="77"/>
+      <c r="I49" s="77"/>
+    </row>
+    <row r="50" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C50" s="77" t="str">
+        <f>CONCATENATE("  EEPROM.write(a, ",P37,"); a++;")</f>
+        <v xml:space="preserve">  EEPROM.write(a, 0); a++;</v>
+      </c>
+      <c r="D50" s="77"/>
+      <c r="E50" s="77"/>
+      <c r="F50" s="77"/>
+      <c r="G50" s="77"/>
+      <c r="H50" s="77"/>
+      <c r="I50" s="77"/>
+    </row>
+    <row r="51" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C51" s="77" t="str">
+        <f>CONCATENATE("  EEPROM.write(a, ",Q37,"); a++;")</f>
+        <v xml:space="preserve">  EEPROM.write(a, 0); a++;</v>
+      </c>
+      <c r="D51" s="77"/>
+      <c r="E51" s="77"/>
+      <c r="F51" s="77"/>
+      <c r="G51" s="77"/>
+      <c r="H51" s="77"/>
+      <c r="I51" s="77"/>
+    </row>
+    <row r="52" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C52" s="77" t="str">
+        <f>CONCATENATE("  EEPROM.write(a, ",R37,"); a++;")</f>
+        <v xml:space="preserve">  EEPROM.write(a, 0); a++;</v>
+      </c>
+      <c r="D52" s="77"/>
+      <c r="E52" s="77"/>
+      <c r="F52" s="77"/>
+      <c r="G52" s="77"/>
+      <c r="H52" s="77"/>
+      <c r="I52" s="77"/>
+    </row>
+    <row r="53" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C53" s="77" t="str">
+        <f>CONCATENATE("  EEPROM.write(a, ",S37,"); a++;")</f>
+        <v xml:space="preserve">  EEPROM.write(a, 0); a++;</v>
+      </c>
+      <c r="D53" s="77"/>
+      <c r="E53" s="77"/>
+      <c r="F53" s="77"/>
+      <c r="G53" s="77"/>
+      <c r="H53" s="77"/>
+      <c r="I53" s="77"/>
+    </row>
+    <row r="54" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C54" s="77" t="str">
+        <f>CONCATENATE("  EEPROM.write(a, ",T37,"); a++;")</f>
+        <v xml:space="preserve">  EEPROM.write(a, 0); a++;</v>
+      </c>
+      <c r="D54" s="77"/>
+      <c r="E54" s="77"/>
+      <c r="F54" s="77"/>
+      <c r="G54" s="77"/>
+      <c r="H54" s="77"/>
+      <c r="I54" s="77"/>
+    </row>
+    <row r="55" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C55" s="77" t="str">
+        <f>CONCATENATE("  EEPROM.write(a, ",U37,"); a++;")</f>
+        <v xml:space="preserve">  EEPROM.write(a, 0); a++;</v>
+      </c>
+      <c r="D55" s="77"/>
+      <c r="E55" s="77"/>
+      <c r="F55" s="77"/>
+      <c r="G55" s="77"/>
+      <c r="H55" s="77"/>
+      <c r="I55" s="77"/>
     </row>
   </sheetData>
-  <mergeCells count="53">
+  <mergeCells count="54">
+    <mergeCell ref="AJ27:AM27"/>
+    <mergeCell ref="O3:Z3"/>
+    <mergeCell ref="AA3:AG3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G4:R4"/>
+    <mergeCell ref="S4:AD4"/>
+    <mergeCell ref="AE4:AG4"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="K5:V5"/>
+    <mergeCell ref="W5:AG5"/>
+    <mergeCell ref="C6:N6"/>
+    <mergeCell ref="O6:Z6"/>
+    <mergeCell ref="AA6:AG6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="G7:R7"/>
+    <mergeCell ref="S7:AD7"/>
+    <mergeCell ref="AE7:AG7"/>
+    <mergeCell ref="B8:J8"/>
+    <mergeCell ref="K8:V8"/>
+    <mergeCell ref="W8:AG8"/>
+    <mergeCell ref="C9:N9"/>
+    <mergeCell ref="O9:Z9"/>
+    <mergeCell ref="AA9:AG9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="G10:R10"/>
+    <mergeCell ref="S10:AD10"/>
+    <mergeCell ref="AE10:AG10"/>
+    <mergeCell ref="B11:J11"/>
+    <mergeCell ref="K11:V11"/>
+    <mergeCell ref="W11:AG11"/>
+    <mergeCell ref="C12:N12"/>
+    <mergeCell ref="O12:Z12"/>
+    <mergeCell ref="AA12:AG12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="G13:R13"/>
+    <mergeCell ref="S13:AD13"/>
+    <mergeCell ref="AE13:AG13"/>
+    <mergeCell ref="B14:J14"/>
+    <mergeCell ref="K14:V14"/>
+    <mergeCell ref="W14:AG14"/>
+    <mergeCell ref="C15:N15"/>
+    <mergeCell ref="O15:Z15"/>
+    <mergeCell ref="AA15:AG15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="G16:R16"/>
+    <mergeCell ref="S16:AD16"/>
+    <mergeCell ref="AE16:AG16"/>
     <mergeCell ref="B19:F19"/>
     <mergeCell ref="B17:J17"/>
     <mergeCell ref="K17:V17"/>
@@ -3066,52 +4494,6 @@
     <mergeCell ref="C18:N18"/>
     <mergeCell ref="O18:Z18"/>
     <mergeCell ref="AA18:AG18"/>
-    <mergeCell ref="C15:N15"/>
-    <mergeCell ref="O15:Z15"/>
-    <mergeCell ref="AA15:AG15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="G16:R16"/>
-    <mergeCell ref="S16:AD16"/>
-    <mergeCell ref="AE16:AG16"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="G13:R13"/>
-    <mergeCell ref="S13:AD13"/>
-    <mergeCell ref="AE13:AG13"/>
-    <mergeCell ref="B14:J14"/>
-    <mergeCell ref="K14:V14"/>
-    <mergeCell ref="W14:AG14"/>
-    <mergeCell ref="B11:J11"/>
-    <mergeCell ref="K11:V11"/>
-    <mergeCell ref="W11:AG11"/>
-    <mergeCell ref="C12:N12"/>
-    <mergeCell ref="O12:Z12"/>
-    <mergeCell ref="AA12:AG12"/>
-    <mergeCell ref="C9:N9"/>
-    <mergeCell ref="O9:Z9"/>
-    <mergeCell ref="AA9:AG9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="G10:R10"/>
-    <mergeCell ref="S10:AD10"/>
-    <mergeCell ref="AE10:AG10"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="G7:R7"/>
-    <mergeCell ref="S7:AD7"/>
-    <mergeCell ref="AE7:AG7"/>
-    <mergeCell ref="B8:J8"/>
-    <mergeCell ref="K8:V8"/>
-    <mergeCell ref="W8:AG8"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="K5:V5"/>
-    <mergeCell ref="W5:AG5"/>
-    <mergeCell ref="C6:N6"/>
-    <mergeCell ref="O6:Z6"/>
-    <mergeCell ref="AA6:AG6"/>
-    <mergeCell ref="O3:Z3"/>
-    <mergeCell ref="AA3:AG3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="G4:R4"/>
-    <mergeCell ref="S4:AD4"/>
-    <mergeCell ref="AE4:AG4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>